<commit_message>
several new data sets added
</commit_message>
<xml_diff>
--- a/pestiziddaten anfragen.xlsx
+++ b/pestiziddaten anfragen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\Uni\projects\PARC\parc_pesticide_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C4D525-8825-4352-8DA2-EF88B6130D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B3611F-F7BC-4A48-825B-01DE32A3C66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>Sachsen</t>
   </si>
@@ -176,6 +176,15 @@
   </si>
   <si>
     <t>Response 18.11.2022 Forwarded to  Landesamt für Naturschutz, Umwelt und Geologie</t>
+  </si>
+  <si>
+    <t>obtained data per email (21.11.22)</t>
+  </si>
+  <si>
+    <t>obtained via email 21.11.22</t>
+  </si>
+  <si>
+    <t>obtained data via email (link to cloud) 22.11.2022</t>
   </si>
 </sst>
 </file>
@@ -525,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,9 +550,10 @@
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42.42578125" customWidth="1"/>
     <col min="8" max="8" width="35.28515625" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -554,7 +564,7 @@
         <v>44855</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -565,8 +575,8 @@
         <v>44855</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -575,8 +585,11 @@
       <c r="C3" s="1">
         <v>44862</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -587,7 +600,7 @@
         <v>44862</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -598,8 +611,8 @@
         <v>44859</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -623,8 +636,11 @@
       <c r="H6" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -635,8 +651,8 @@
         <v>44862</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
@@ -651,8 +667,11 @@
       <c r="E8" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -663,7 +682,7 @@
         <v>44860</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
@@ -677,7 +696,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
@@ -688,7 +707,7 @@
         <v>44860</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
@@ -699,7 +718,7 @@
         <v>44862</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>

</xml_diff>